<commit_message>
Added licence entry for new icon library in third-party
</commit_message>
<xml_diff>
--- a/Documentation/Open Twin Licenses.xlsx
+++ b/Documentation/Open Twin Licenses.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Daten\Forschung\Forschungskooperationen\Bosch\2020-11-22 Überarbeitetes Angebot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OpenTwin\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CC24BE8-D6CE-4567-9E77-7A5F1520A444}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AA9E364-BC43-4407-95A6-80579AA50661}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5625" yWindow="690" windowWidth="51885" windowHeight="21990" xr2:uid="{B35B6C7E-C187-470B-817D-DD7F165A6147}"/>
+    <workbookView xWindow="5628" yWindow="696" windowWidth="51888" windowHeight="21996" xr2:uid="{B35B6C7E-C187-470B-817D-DD7F165A6147}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -20,21 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="109">
   <si>
     <t>Apple Public Source License, Version 2.0, 6. August 2003</t>
   </si>
@@ -355,6 +346,12 @@
   </si>
   <si>
     <t>Open Twin (all components)</t>
+  </si>
+  <si>
+    <t>IconPark</t>
+  </si>
+  <si>
+    <t>github.com/bytedance/IconPark</t>
   </si>
 </sst>
 </file>
@@ -685,65 +682,65 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1062,24 +1059,24 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:H30"/>
+  <dimension ref="B1:H31"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K34" sqref="K34"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="33.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.28515625" customWidth="1"/>
-    <col min="6" max="6" width="45.42578125" customWidth="1"/>
-    <col min="7" max="7" width="9.85546875" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" customWidth="1"/>
+    <col min="3" max="3" width="33.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.33203125" customWidth="1"/>
+    <col min="6" max="6" width="45.44140625" customWidth="1"/>
+    <col min="7" max="7" width="9.88671875" customWidth="1"/>
+    <col min="8" max="8" width="10.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C2" s="2" t="s">
         <v>32</v>
       </c>
@@ -1099,7 +1096,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="2:8" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:8" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C3" s="6" t="s">
         <v>106</v>
       </c>
@@ -1119,578 +1116,599 @@
         <v>104</v>
       </c>
     </row>
-    <row r="4" spans="2:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="B4" s="9" t="s">
+    <row r="4" spans="2:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B4" s="26" t="s">
         <v>105</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="10">
         <v>452</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="G4" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="H4" s="14" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="2:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="15"/>
-      <c r="C5" s="16" t="s">
+      <c r="H4" s="13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="27"/>
+      <c r="C5" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D5" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="18" t="s">
+      <c r="E5" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="F5" s="18" t="s">
+      <c r="F5" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="G5" s="17" t="s">
+      <c r="G5" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="H5" s="19" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="15"/>
-      <c r="C6" s="16" t="s">
+      <c r="H5" s="17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B6" s="27"/>
+      <c r="C6" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="D6" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="E6" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="18" t="s">
+      <c r="F6" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="G6" s="17" t="s">
+      <c r="G6" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="H6" s="19" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="15"/>
-      <c r="C7" s="16" t="s">
+      <c r="H6" s="17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B7" s="27"/>
+      <c r="C7" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="D7" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="E7" s="18" t="s">
+      <c r="E7" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="F7" s="18" t="s">
+      <c r="F7" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="G7" s="17" t="s">
+      <c r="G7" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="H7" s="19" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="15"/>
-      <c r="C8" s="16" t="s">
+      <c r="H7" s="17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B8" s="27"/>
+      <c r="C8" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="20" t="s">
+      <c r="D8" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="E8" s="18" t="s">
+      <c r="E8" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="F8" s="18" t="s">
+      <c r="F8" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="G8" s="17" t="s">
+      <c r="G8" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="H8" s="19" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="15"/>
-      <c r="C9" s="16" t="s">
+      <c r="H8" s="17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="27"/>
+      <c r="C9" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="20" t="s">
+      <c r="D9" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="E9" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="F9" s="18" t="s">
+      <c r="F9" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="G9" s="17" t="s">
+      <c r="G9" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="H9" s="19" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="15"/>
-      <c r="C10" s="16" t="s">
+      <c r="H9" s="17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B10" s="27"/>
+      <c r="C10" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="D10" s="20" t="s">
+      <c r="D10" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="E10" s="18" t="s">
+      <c r="E10" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="F10" s="18" t="s">
+      <c r="F10" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="G10" s="17" t="s">
+      <c r="G10" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="H10" s="19" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="15"/>
-      <c r="C11" s="16" t="s">
+      <c r="H10" s="17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B11" s="27"/>
+      <c r="C11" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="D11" s="20" t="s">
+      <c r="D11" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="E11" s="18" t="s">
+      <c r="E11" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="F11" s="18" t="s">
+      <c r="F11" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="G11" s="17" t="s">
+      <c r="G11" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="H11" s="19" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="15"/>
-      <c r="C12" s="16" t="s">
+      <c r="H11" s="17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B12" s="27"/>
+      <c r="C12" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="20" t="s">
+      <c r="D12" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="E12" s="18" t="s">
+      <c r="E12" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="F12" s="18" t="s">
+      <c r="F12" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="G12" s="17" t="s">
+      <c r="G12" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="H12" s="19" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="15"/>
-      <c r="C13" s="16" t="s">
+      <c r="H12" s="17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B13" s="27"/>
+      <c r="C13" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="21" t="s">
+      <c r="D13" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="E13" s="18" t="s">
+      <c r="E13" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="F13" s="18" t="s">
+      <c r="F13" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="G13" s="17" t="s">
+      <c r="G13" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="H13" s="19" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="15"/>
-      <c r="C14" s="16" t="s">
+      <c r="H13" s="17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B14" s="27"/>
+      <c r="C14" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D14" s="20" t="s">
+      <c r="D14" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="E14" s="18" t="s">
+      <c r="E14" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="F14" s="18" t="s">
+      <c r="F14" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="G14" s="17" t="s">
+      <c r="G14" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="H14" s="19" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="15"/>
-      <c r="C15" s="16" t="s">
+      <c r="H14" s="17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B15" s="27"/>
+      <c r="C15" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="21" t="s">
+      <c r="D15" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="E15" s="18" t="s">
+      <c r="E15" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="F15" s="18" t="s">
+      <c r="F15" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="G15" s="17" t="s">
+      <c r="G15" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="H15" s="19" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="16" spans="2:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="15"/>
-      <c r="C16" s="16" t="s">
+      <c r="H15" s="17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="27"/>
+      <c r="C16" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="D16" s="20" t="s">
+      <c r="D16" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="E16" s="18" t="s">
+      <c r="E16" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="F16" s="18" t="s">
+      <c r="F16" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="G16" s="17" t="s">
+      <c r="G16" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="H16" s="19" t="s">
+      <c r="H16" s="17" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="15"/>
-      <c r="C17" s="16" t="s">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B17" s="27"/>
+      <c r="C17" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="D17" s="21" t="s">
+      <c r="D17" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="E17" s="18" t="s">
+      <c r="E17" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="F17" s="18" t="s">
+      <c r="F17" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="G17" s="17" t="s">
+      <c r="G17" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="H17" s="19" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B18" s="15"/>
-      <c r="C18" s="16" t="s">
+      <c r="H17" s="17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B18" s="27"/>
+      <c r="C18" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="D18" s="21" t="s">
+      <c r="D18" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="E18" s="18" t="s">
+      <c r="E18" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="F18" s="18" t="s">
+      <c r="F18" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="G18" s="17" t="s">
+      <c r="G18" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="H18" s="19" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B19" s="15"/>
-      <c r="C19" s="16" t="s">
+      <c r="H18" s="17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B19" s="27"/>
+      <c r="C19" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="D19" s="20" t="s">
+      <c r="D19" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="E19" s="18" t="s">
+      <c r="E19" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="F19" s="18" t="s">
+      <c r="F19" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="G19" s="17" t="s">
+      <c r="G19" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="H19" s="19" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B20" s="15"/>
-      <c r="C20" s="16" t="s">
+      <c r="H19" s="17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B20" s="27"/>
+      <c r="C20" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="D20" s="20" t="s">
+      <c r="D20" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="E20" s="18" t="s">
+      <c r="E20" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="F20" s="18" t="s">
+      <c r="F20" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="G20" s="17" t="s">
+      <c r="G20" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="H20" s="19" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="15"/>
-      <c r="C21" s="16" t="s">
+      <c r="H20" s="17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B21" s="27"/>
+      <c r="C21" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="D21" s="22" t="s">
+      <c r="D21" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="E21" s="18" t="s">
+      <c r="E21" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="F21" s="18" t="s">
+      <c r="F21" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="G21" s="17" t="s">
+      <c r="G21" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="H21" s="19" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="15"/>
-      <c r="C22" s="16" t="s">
+      <c r="H21" s="17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="27"/>
+      <c r="C22" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="D22" s="17" t="s">
+      <c r="D22" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="E22" s="18" t="s">
+      <c r="E22" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="F22" s="18" t="s">
+      <c r="F22" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="G22" s="17" t="s">
+      <c r="G22" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="H22" s="19" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="23" spans="2:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="15"/>
-      <c r="C23" s="16" t="s">
+      <c r="H22" s="17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="27"/>
+      <c r="C23" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="D23" s="17" t="s">
+      <c r="D23" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="E23" s="18" t="s">
+      <c r="E23" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="F23" s="18" t="s">
+      <c r="F23" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="G23" s="17" t="s">
+      <c r="G23" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="H23" s="19" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="24" spans="2:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="15"/>
-      <c r="C24" s="16" t="s">
+      <c r="H23" s="17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="27"/>
+      <c r="C24" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="D24" s="17" t="s">
+      <c r="D24" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="E24" s="18" t="s">
+      <c r="E24" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="F24" s="18" t="s">
+      <c r="F24" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="G24" s="17" t="s">
+      <c r="G24" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="H24" s="19" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="25" spans="2:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="15"/>
-      <c r="C25" s="16" t="s">
+      <c r="H24" s="17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="27"/>
+      <c r="C25" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="D25" s="20" t="s">
+      <c r="D25" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="E25" s="18" t="s">
+      <c r="E25" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="F25" s="18" t="s">
+      <c r="F25" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="G25" s="17" t="s">
+      <c r="G25" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="H25" s="19" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="26" spans="2:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="15"/>
-      <c r="C26" s="16" t="s">
+      <c r="H25" s="17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="27"/>
+      <c r="C26" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="D26" s="20" t="s">
+      <c r="D26" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="E26" s="18" t="s">
+      <c r="E26" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="F26" s="18" t="s">
+      <c r="F26" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="G26" s="17" t="s">
+      <c r="G26" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="H26" s="19" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="27" spans="2:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="15"/>
-      <c r="C27" s="16" t="s">
+      <c r="H26" s="17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="27"/>
+      <c r="C27" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="D27" s="20" t="s">
+      <c r="D27" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="E27" s="18" t="s">
+      <c r="E27" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="F27" s="18" t="s">
+      <c r="F27" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="G27" s="17" t="s">
+      <c r="G27" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="H27" s="19" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="28" spans="2:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="15"/>
-      <c r="C28" s="16" t="s">
+      <c r="H27" s="17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="27"/>
+      <c r="C28" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="D28" s="20" t="s">
+      <c r="D28" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="E28" s="18" t="s">
+      <c r="E28" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="F28" s="18" t="s">
+      <c r="F28" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="G28" s="17" t="s">
+      <c r="G28" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="H28" s="19" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="29" spans="2:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="15"/>
-      <c r="C29" s="16" t="s">
+      <c r="H28" s="17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="27"/>
+      <c r="C29" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="D29" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="E29" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="F29" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="G29" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="H29" s="17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="27"/>
+      <c r="C30" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="D29" s="20" t="s">
+      <c r="D30" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="E29" s="18" t="s">
+      <c r="E30" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="F29" s="18" t="s">
+      <c r="F30" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="G29" s="17" t="s">
+      <c r="G30" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="H29" s="19" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="30" spans="2:8" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="23"/>
-      <c r="C30" s="24" t="s">
+      <c r="H30" s="17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B31" s="28"/>
+      <c r="C31" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="D30" s="25">
+      <c r="D31" s="22">
         <v>2017</v>
       </c>
-      <c r="E30" s="26" t="s">
+      <c r="E31" s="23" t="s">
         <v>95</v>
       </c>
-      <c r="F30" s="26" t="s">
+      <c r="F31" s="23" t="s">
         <v>96</v>
       </c>
-      <c r="G30" s="27" t="s">
+      <c r="G31" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="H30" s="28" t="s">
+      <c r="H31" s="25" t="s">
         <v>38</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B4:B30"/>
+    <mergeCell ref="B4:B31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="75" orientation="landscape" r:id="rId1"/>

</xml_diff>